<commit_message>
augh, spreadsheet migration no fun
</commit_message>
<xml_diff>
--- a/applications/default/data/national/default_options.xlsx
+++ b/applications/default/data/national/default_options.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/default/data/national/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E16A01F7-753E-8444-847F-97F935C2A588}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{3C28A406-3B38-3B44-81A1-855DF4E1C8BA}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="12795" windowHeight="15540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Programs to include" sheetId="3" r:id="rId1"/>
     <sheet name="Coverage scenario" sheetId="12" r:id="rId2"/>
     <sheet name="Budget scenario" sheetId="11" r:id="rId3"/>
-    <sheet name="Optimisation options" sheetId="13" r:id="rId4"/>
+    <sheet name="Optimization options" sheetId="13" r:id="rId4"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId5"/>
@@ -216,7 +210,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -346,7 +340,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{84516AC3-0F6C-C446-9516-6FDA12772B8D}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -548,7 +542,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -600,7 +594,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -794,31 +788,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9848D68B-8BFC-1547-A075-485AE6A3F40F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56" style="5" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -826,25 +820,25 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>31</v>
       </c>
@@ -852,13 +846,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -866,43 +860,43 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>43</v>
       </c>
@@ -910,13 +904,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
@@ -924,13 +918,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>7</v>
       </c>
@@ -938,43 +932,43 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>17</v>
       </c>
@@ -982,25 +976,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>16</v>
       </c>
@@ -1008,7 +1002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>15</v>
       </c>
@@ -1016,37 +1010,37 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>9</v>
       </c>
@@ -1054,7 +1048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>8</v>
       </c>
@@ -1070,7 +1064,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF98E75-2B9A-1140-998D-A6BF823A844A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1080,14 +1074,14 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="5"/>
-    <col min="3" max="4" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="10.875" style="5"/>
+    <col min="3" max="4" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1142,7 +1136,7 @@
       <c r="AD1" s="2"/>
       <c r="AE1" s="2"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -1159,7 +1153,7 @@
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
@@ -1176,7 +1170,7 @@
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
@@ -1193,7 +1187,7 @@
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>31</v>
       </c>
@@ -1210,7 +1204,7 @@
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -1227,7 +1221,7 @@
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1244,7 +1238,7 @@
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1261,7 +1255,7 @@
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
@@ -1278,7 +1272,7 @@
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>44</v>
       </c>
@@ -1295,7 +1289,7 @@
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>45</v>
       </c>
@@ -1312,7 +1306,7 @@
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>46</v>
       </c>
@@ -1329,7 +1323,7 @@
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>47</v>
       </c>
@@ -1346,7 +1340,7 @@
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>43</v>
       </c>
@@ -1365,7 +1359,7 @@
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>48</v>
       </c>
@@ -1382,7 +1376,7 @@
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
@@ -1399,7 +1393,7 @@
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
@@ -1416,7 +1410,7 @@
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>7</v>
       </c>
@@ -1435,7 +1429,7 @@
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>6</v>
       </c>
@@ -1452,7 +1446,7 @@
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>4</v>
       </c>
@@ -1469,7 +1463,7 @@
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
@@ -1486,7 +1480,7 @@
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -1503,7 +1497,7 @@
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>23</v>
       </c>
@@ -1520,7 +1514,7 @@
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
@@ -1537,7 +1531,7 @@
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>17</v>
       </c>
@@ -1554,7 +1548,7 @@
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>21</v>
       </c>
@@ -1571,7 +1565,7 @@
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>20</v>
       </c>
@@ -1588,7 +1582,7 @@
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>19</v>
       </c>
@@ -1605,7 +1599,7 @@
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>16</v>
       </c>
@@ -1624,7 +1618,7 @@
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>15</v>
       </c>
@@ -1643,7 +1637,7 @@
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>14</v>
       </c>
@@ -1660,7 +1654,7 @@
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>13</v>
       </c>
@@ -1677,7 +1671,7 @@
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>12</v>
       </c>
@@ -1694,7 +1688,7 @@
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>11</v>
       </c>
@@ -1711,7 +1705,7 @@
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>10</v>
       </c>
@@ -1728,7 +1722,7 @@
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>9</v>
       </c>
@@ -1745,7 +1739,7 @@
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>8</v>
       </c>
@@ -1762,7 +1756,7 @@
       <c r="J37" s="13"/>
       <c r="K37" s="13"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="7"/>
@@ -1783,7 +1777,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8FFD43-0A0F-4D4C-8EFD-D178D6D096FB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1793,15 +1787,15 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="5"/>
-    <col min="3" max="4" width="10.83203125" style="1"/>
-    <col min="12" max="12" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="10.875" style="5"/>
+    <col min="3" max="4" width="10.875" style="1"/>
+    <col min="12" max="12" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1844,7 +1838,7 @@
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -1861,7 +1855,7 @@
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
@@ -1878,7 +1872,7 @@
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
@@ -1895,7 +1889,7 @@
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>31</v>
       </c>
@@ -1912,7 +1906,7 @@
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -1929,7 +1923,7 @@
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1946,7 +1940,7 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1963,7 +1957,7 @@
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
@@ -1980,7 +1974,7 @@
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>44</v>
       </c>
@@ -1997,7 +1991,7 @@
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>45</v>
       </c>
@@ -2014,7 +2008,7 @@
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>46</v>
       </c>
@@ -2031,7 +2025,7 @@
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>47</v>
       </c>
@@ -2048,7 +2042,7 @@
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>43</v>
       </c>
@@ -2065,7 +2059,7 @@
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>48</v>
       </c>
@@ -2082,7 +2076,7 @@
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
@@ -2099,7 +2093,7 @@
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
@@ -2116,7 +2110,7 @@
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>7</v>
       </c>
@@ -2133,7 +2127,7 @@
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>6</v>
       </c>
@@ -2150,7 +2144,7 @@
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>4</v>
       </c>
@@ -2167,7 +2161,7 @@
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
@@ -2184,7 +2178,7 @@
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -2201,7 +2195,7 @@
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>23</v>
       </c>
@@ -2218,7 +2212,7 @@
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
@@ -2235,7 +2229,7 @@
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>17</v>
       </c>
@@ -2252,7 +2246,7 @@
       <c r="J25" s="16"/>
       <c r="K25" s="16"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>21</v>
       </c>
@@ -2269,7 +2263,7 @@
       <c r="J26" s="16"/>
       <c r="K26" s="16"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>20</v>
       </c>
@@ -2286,7 +2280,7 @@
       <c r="J27" s="16"/>
       <c r="K27" s="16"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>19</v>
       </c>
@@ -2303,7 +2297,7 @@
       <c r="J28" s="16"/>
       <c r="K28" s="16"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>16</v>
       </c>
@@ -2320,7 +2314,7 @@
       <c r="J29" s="16"/>
       <c r="K29" s="16"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>15</v>
       </c>
@@ -2337,7 +2331,7 @@
       <c r="J30" s="16"/>
       <c r="K30" s="16"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>14</v>
       </c>
@@ -2354,7 +2348,7 @@
       <c r="J31" s="16"/>
       <c r="K31" s="16"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>13</v>
       </c>
@@ -2371,7 +2365,7 @@
       <c r="J32" s="16"/>
       <c r="K32" s="16"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>12</v>
       </c>
@@ -2388,7 +2382,7 @@
       <c r="J33" s="16"/>
       <c r="K33" s="16"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>11</v>
       </c>
@@ -2405,7 +2399,7 @@
       <c r="J34" s="16"/>
       <c r="K34" s="16"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>10</v>
       </c>
@@ -2422,7 +2416,7 @@
       <c r="J35" s="16"/>
       <c r="K35" s="16"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>9</v>
       </c>
@@ -2439,7 +2433,7 @@
       <c r="J36" s="16"/>
       <c r="K36" s="16"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>8</v>
       </c>
@@ -2456,7 +2450,7 @@
       <c r="J37" s="16"/>
       <c r="K37" s="16"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="7"/>
@@ -2477,24 +2471,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84CE95BA-2BE6-BA4F-A839-A87510FDB8B4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.875" customWidth="1"/>
+    <col min="5" max="5" width="14.375" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>39</v>
       </c>
@@ -2517,7 +2511,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>2017</v>
       </c>

</xml_diff>

<commit_message>
Removed Birth age program from all books, removed IYCF 2&3 from default books
</commit_message>
<xml_diff>
--- a/applications/default/data/national/default_options.xlsx
+++ b/applications/default/data/national/default_options.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/default/data/national/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6E657738-082C-FD4D-B176-991B1A67DC5B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="12795" windowHeight="15540" activeTab="3"/>
+    <workbookView xWindow="13020" yWindow="-21140" windowWidth="19200" windowHeight="21140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Programs to include" sheetId="3" r:id="rId1"/>
@@ -49,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="49">
   <si>
     <t>Coverage</t>
   </si>
@@ -63,15 +69,9 @@
     <t>Program</t>
   </si>
   <si>
-    <t>IYCF 3</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
-    <t>IYCF 2</t>
-  </si>
-  <si>
     <t>IYCF 1</t>
   </si>
   <si>
@@ -150,9 +150,6 @@
     <t>Calcium supplementation</t>
   </si>
   <si>
-    <t>Birth age program</t>
-  </si>
-  <si>
     <t>Balanced energy-protein supplementation</t>
   </si>
   <si>
@@ -204,13 +201,13 @@
     <t>1,2</t>
   </si>
   <si>
-    <t>thrive, child_deaths</t>
+    <t>thrive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -340,7 +337,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -788,275 +785,257 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="56" style="5" customWidth="1"/>
-    <col min="2" max="2" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="4"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="4"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="4"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="4"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="B29" s="4"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="B30" s="4"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="4"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="4"/>
-    </row>
   </sheetData>
-  <sortState ref="A2:B37">
-    <sortCondition ref="A2:A37"/>
+  <sortState ref="A2:B34">
+    <sortCondition ref="A2:A34"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1064,24 +1043,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AE38"/>
+  <dimension ref="A1:AE35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="5"/>
-    <col min="3" max="4" width="10.875" style="1"/>
+    <col min="2" max="2" width="10.83203125" style="5"/>
+    <col min="3" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1136,9 +1115,9 @@
       <c r="AD1" s="2"/>
       <c r="AE1" s="2"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -1153,9 +1132,9 @@
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>0</v>
@@ -1170,9 +1149,9 @@
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>0</v>
@@ -1187,9 +1166,9 @@
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>0</v>
@@ -1204,9 +1183,9 @@
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>0</v>
@@ -1221,9 +1200,9 @@
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>0</v>
@@ -1238,9 +1217,9 @@
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>0</v>
@@ -1255,9 +1234,9 @@
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>27</v>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>0</v>
@@ -1272,9 +1251,9 @@
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>0</v>
@@ -1289,9 +1268,9 @@
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>0</v>
@@ -1306,9 +1285,9 @@
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>0</v>
@@ -1323,15 +1302,17 @@
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>47</v>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="D13" s="13">
+        <v>0.95</v>
+      </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
@@ -1340,17 +1321,15 @@
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="13"/>
-      <c r="D14" s="13">
-        <v>0.95</v>
-      </c>
+      <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -1359,9 +1338,9 @@
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>0</v>
@@ -1376,9 +1355,9 @@
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>0</v>
@@ -1393,15 +1372,17 @@
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="D17" s="13">
+        <v>0.95</v>
+      </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
@@ -1410,17 +1391,15 @@
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="13"/>
-      <c r="D18" s="13">
-        <v>0.95</v>
-      </c>
+      <c r="D18" s="13"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
@@ -1429,9 +1408,9 @@
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>0</v>
@@ -1446,9 +1425,9 @@
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>0</v>
@@ -1463,9 +1442,9 @@
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>0</v>
@@ -1480,9 +1459,9 @@
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>0</v>
@@ -1497,9 +1476,9 @@
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>0</v>
@@ -1514,9 +1493,9 @@
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>0</v>
@@ -1531,7 +1510,7 @@
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>17</v>
       </c>
@@ -1548,15 +1527,17 @@
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
+      <c r="D26" s="13">
+        <v>0.95</v>
+      </c>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
@@ -1565,15 +1546,17 @@
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
+      <c r="D27" s="13">
+        <v>0.95</v>
+      </c>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
@@ -1582,9 +1565,9 @@
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>0</v>
@@ -1599,17 +1582,15 @@
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="13"/>
-      <c r="D29" s="13">
-        <v>0.95</v>
-      </c>
+      <c r="D29" s="13"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
@@ -1618,17 +1599,15 @@
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="13"/>
-      <c r="D30" s="13">
-        <v>0.95</v>
-      </c>
+      <c r="D30" s="13"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
@@ -1637,9 +1616,9 @@
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>0</v>
@@ -1654,9 +1633,9 @@
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>0</v>
@@ -1671,9 +1650,9 @@
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>0</v>
@@ -1688,9 +1667,9 @@
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>0</v>
@@ -1705,71 +1684,20 @@
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A2:K37">
-    <sortCondition ref="A2:A37"/>
+  <sortState ref="A2:K34">
+    <sortCondition ref="A2:A34"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1777,25 +1705,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:S38"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="5"/>
-    <col min="3" max="4" width="10.875" style="1"/>
-    <col min="12" max="12" width="10.875" style="1"/>
+    <col min="2" max="2" width="10.83203125" style="5"/>
+    <col min="3" max="4" width="10.83203125" style="1"/>
+    <col min="12" max="12" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1838,9 +1766,9 @@
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -1855,9 +1783,9 @@
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>1</v>
@@ -1872,9 +1800,9 @@
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>1</v>
@@ -1889,9 +1817,9 @@
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>1</v>
@@ -1906,9 +1834,9 @@
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>1</v>
@@ -1923,9 +1851,9 @@
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>1</v>
@@ -1940,9 +1868,9 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>1</v>
@@ -1957,9 +1885,9 @@
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>27</v>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>1</v>
@@ -1974,9 +1902,9 @@
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>1</v>
@@ -1991,9 +1919,9 @@
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>1</v>
@@ -2008,9 +1936,9 @@
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>1</v>
@@ -2025,9 +1953,9 @@
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>47</v>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>1</v>
@@ -2042,9 +1970,9 @@
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>1</v>
@@ -2059,9 +1987,9 @@
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>1</v>
@@ -2076,9 +2004,9 @@
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>1</v>
@@ -2093,9 +2021,9 @@
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>1</v>
@@ -2110,9 +2038,9 @@
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>1</v>
@@ -2127,9 +2055,9 @@
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>1</v>
@@ -2144,9 +2072,9 @@
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>1</v>
@@ -2161,9 +2089,9 @@
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>1</v>
@@ -2178,9 +2106,9 @@
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>1</v>
@@ -2195,9 +2123,9 @@
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>1</v>
@@ -2212,9 +2140,9 @@
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>1</v>
@@ -2229,7 +2157,7 @@
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>17</v>
       </c>
@@ -2246,9 +2174,9 @@
       <c r="J25" s="16"/>
       <c r="K25" s="16"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>1</v>
@@ -2263,9 +2191,9 @@
       <c r="J26" s="16"/>
       <c r="K26" s="16"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>1</v>
@@ -2280,9 +2208,9 @@
       <c r="J27" s="16"/>
       <c r="K27" s="16"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>1</v>
@@ -2297,9 +2225,9 @@
       <c r="J28" s="16"/>
       <c r="K28" s="16"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>1</v>
@@ -2314,9 +2242,9 @@
       <c r="J29" s="16"/>
       <c r="K29" s="16"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>1</v>
@@ -2331,9 +2259,9 @@
       <c r="J30" s="16"/>
       <c r="K30" s="16"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>1</v>
@@ -2348,9 +2276,9 @@
       <c r="J31" s="16"/>
       <c r="K31" s="16"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>1</v>
@@ -2365,9 +2293,9 @@
       <c r="J32" s="16"/>
       <c r="K32" s="16"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>1</v>
@@ -2382,9 +2310,9 @@
       <c r="J33" s="16"/>
       <c r="K33" s="16"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>1</v>
@@ -2399,71 +2327,20 @@
       <c r="J34" s="16"/>
       <c r="K34" s="16"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="16"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A2:K37">
-    <sortCondition ref="A2:A37"/>
+  <sortState ref="A2:K34">
+    <sortCondition ref="A2:A34"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2471,47 +2348,48 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="13.875" customWidth="1"/>
-    <col min="5" max="5" width="14.375" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>2017</v>
       </c>
@@ -2519,19 +2397,19 @@
         <v>2025</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E2" s="11">
-        <v>10000000</v>
+        <v>5000000</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>